<commit_message>
added libcsp/ XTEA for comparison
</commit_message>
<xml_diff>
--- a/results/kyber_performance_stats.xlsx
+++ b/results/kyber_performance_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\FHNW\QSIT\fhnw-ise-qcrypt\kyber-benchmarks-STM32F4\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6949403-92F7-48AC-AA53-2D91452BDAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B903F63D-B148-4A78-A4E1-6F913E4E4F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{0FA4A56B-E400-4D81-B285-E4F07F5EA511}"/>
   </bookViews>
@@ -4380,7 +4380,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-CH"/>
-              <a:t>kyber-768 performance</a:t>
+              <a:t>kyber-512 performance</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="de-CH"/>
@@ -4933,7 +4933,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-CH"/>
-              <a:t>kyber-1024 performance</a:t>
+              <a:t>kyber-512 performance</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="de-CH"/>
@@ -12635,8 +12635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE64E7BF-33F8-48FD-AC4F-26F197E7DDD2}">
   <dimension ref="A4:AF159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="W94" sqref="W94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12874,11 +12874,11 @@
         <v>1.2408333333333335</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" ref="I10:I32" si="2">E10/B10</f>
+        <f t="shared" ref="I10:I33" si="2">E10/B10</f>
         <v>43.834314550042052</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ref="J10:J32" si="3">F10/C10</f>
+        <f t="shared" ref="J10:J33" si="3">F10/C10</f>
         <v>44.090524534686971</v>
       </c>
       <c r="M10">
@@ -15517,15 +15517,15 @@
         <v>39</v>
       </c>
       <c r="B98" s="9">
-        <f t="shared" ref="B98:B106" si="24">C39</f>
+        <f>C39</f>
         <v>4013592</v>
       </c>
       <c r="C98" s="9">
-        <f t="shared" ref="C98:C106" si="25">N39</f>
+        <f>N39</f>
         <v>1476327</v>
       </c>
       <c r="D98" s="9">
-        <f t="shared" ref="D98:D106" si="26">Y39</f>
+        <f>Y39</f>
         <v>212259</v>
       </c>
     </row>
@@ -15534,15 +15534,15 @@
         <v>40</v>
       </c>
       <c r="B99" s="9">
-        <f t="shared" si="24"/>
+        <f>C40</f>
         <v>575006</v>
       </c>
       <c r="C99" s="9">
-        <f t="shared" si="25"/>
+        <f>N40</f>
         <v>3331994</v>
       </c>
       <c r="D99" s="9">
-        <f t="shared" si="26"/>
+        <f>Y40</f>
         <v>2250365</v>
       </c>
     </row>
@@ -15551,15 +15551,15 @@
         <v>41</v>
       </c>
       <c r="B100" s="9">
-        <f t="shared" si="24"/>
+        <f>C41</f>
         <v>905256</v>
       </c>
       <c r="C100" s="9">
-        <f t="shared" si="25"/>
+        <f>N41</f>
         <v>3524569</v>
       </c>
       <c r="D100" s="9">
-        <f t="shared" si="26"/>
+        <f>Y41</f>
         <v>2675360</v>
       </c>
     </row>
@@ -15568,15 +15568,15 @@
         <v>42</v>
       </c>
       <c r="B101" s="9">
-        <f t="shared" si="24"/>
+        <f>C42</f>
         <v>289139</v>
       </c>
       <c r="C101" s="9">
-        <f t="shared" si="25"/>
+        <f>N42</f>
         <v>509012</v>
       </c>
       <c r="D101" s="9">
-        <f t="shared" si="26"/>
+        <f>Y42</f>
         <v>2462962</v>
       </c>
     </row>
@@ -15585,15 +15585,15 @@
         <v>44</v>
       </c>
       <c r="B102" s="9">
-        <f t="shared" si="24"/>
+        <f>C43</f>
         <v>1571707</v>
       </c>
       <c r="C102" s="9">
-        <f t="shared" si="25"/>
+        <f>N43</f>
         <v>2633480</v>
       </c>
       <c r="D102" s="9">
-        <f t="shared" si="26"/>
+        <f>Y43</f>
         <v>709290</v>
       </c>
     </row>
@@ -15602,15 +15602,15 @@
         <v>43</v>
       </c>
       <c r="B103" s="9">
-        <f t="shared" si="24"/>
+        <f>C44</f>
         <v>996807</v>
       </c>
       <c r="C103" s="9">
-        <f t="shared" si="25"/>
+        <f>N44</f>
         <v>3602926</v>
       </c>
       <c r="D103" s="9">
-        <f t="shared" si="26"/>
+        <f>Y44</f>
         <v>2756685</v>
       </c>
     </row>
@@ -15619,15 +15619,15 @@
         <v>45</v>
       </c>
       <c r="B104" s="9">
-        <f t="shared" si="24"/>
+        <f>C45</f>
         <v>288038</v>
       </c>
       <c r="C104" s="9">
-        <f t="shared" si="25"/>
+        <f>N45</f>
         <v>508262</v>
       </c>
       <c r="D104" s="9">
-        <f t="shared" si="26"/>
+        <f>Y45</f>
         <v>2463179</v>
       </c>
     </row>
@@ -15636,15 +15636,15 @@
         <v>46</v>
       </c>
       <c r="B105" s="9">
-        <f t="shared" si="24"/>
+        <f>C46</f>
         <v>2145910</v>
       </c>
       <c r="C105" s="9">
-        <f t="shared" si="25"/>
+        <f>N46</f>
         <v>1808350</v>
       </c>
       <c r="D105" s="9">
-        <f t="shared" si="26"/>
+        <f>Y46</f>
         <v>3116057</v>
       </c>
     </row>
@@ -15653,15 +15653,15 @@
         <v>47</v>
       </c>
       <c r="B106" s="9">
-        <f t="shared" si="24"/>
+        <f>C47</f>
         <v>1898326</v>
       </c>
       <c r="C106" s="9">
-        <f t="shared" si="25"/>
+        <f>N47</f>
         <v>2957516</v>
       </c>
       <c r="D106" s="9">
-        <f t="shared" si="26"/>
+        <f>Y47</f>
         <v>1291641</v>
       </c>
     </row>
@@ -15686,15 +15686,15 @@
         <v>39</v>
       </c>
       <c r="B111" s="9">
-        <f t="shared" ref="B111:B119" si="27">F39</f>
+        <f>F39</f>
         <v>4011162</v>
       </c>
       <c r="C111" s="9">
-        <f t="shared" ref="C111:C119" si="28">Q39</f>
+        <f>Q39</f>
         <v>5770662</v>
       </c>
       <c r="D111" s="9">
-        <f t="shared" ref="D111:D119" si="29">AB39</f>
+        <f>AB39</f>
         <v>8801144</v>
       </c>
     </row>
@@ -15703,15 +15703,15 @@
         <v>40</v>
       </c>
       <c r="B112" s="9">
-        <f t="shared" si="27"/>
+        <f>F40</f>
         <v>4874271</v>
       </c>
       <c r="C112" s="9">
-        <f t="shared" si="28"/>
+        <f>Q40</f>
         <v>7631256</v>
       </c>
       <c r="D112" s="9">
-        <f t="shared" si="29"/>
+        <f>AB40</f>
         <v>10848911</v>
       </c>
     </row>
@@ -15720,15 +15720,15 @@
         <v>41</v>
       </c>
       <c r="B113" s="9">
-        <f t="shared" si="27"/>
+        <f>F41</f>
         <v>5204524</v>
       </c>
       <c r="C113" s="9">
-        <f t="shared" si="28"/>
+        <f>Q41</f>
         <v>7823831</v>
       </c>
       <c r="D113" s="9">
-        <f t="shared" si="29"/>
+        <f>AB41</f>
         <v>11273893</v>
       </c>
     </row>
@@ -15737,15 +15737,15 @@
         <v>42</v>
       </c>
       <c r="B114" s="9">
-        <f t="shared" si="27"/>
+        <f>F42</f>
         <v>8884219</v>
       </c>
       <c r="C114" s="9">
-        <f t="shared" si="28"/>
+        <f>Q42</f>
         <v>13400542</v>
       </c>
       <c r="D114" s="9">
-        <f t="shared" si="29"/>
+        <f>AB42</f>
         <v>19650115</v>
       </c>
     </row>
@@ -15754,15 +15754,15 @@
         <v>44</v>
       </c>
       <c r="B115" s="9">
-        <f t="shared" si="27"/>
+        <f>F43</f>
         <v>10170245</v>
       </c>
       <c r="C115" s="9">
-        <f t="shared" si="28"/>
+        <f>Q43</f>
         <v>15531274</v>
       </c>
       <c r="D115" s="9">
-        <f t="shared" si="29"/>
+        <f>AB43</f>
         <v>22205635</v>
       </c>
     </row>
@@ -15771,15 +15771,15 @@
         <v>43</v>
       </c>
       <c r="B116" s="9">
-        <f t="shared" si="27"/>
+        <f>F44</f>
         <v>5296074</v>
       </c>
       <c r="C116" s="9">
-        <f t="shared" si="28"/>
+        <f>Q44</f>
         <v>7902191</v>
       </c>
       <c r="D116" s="9">
-        <f t="shared" si="29"/>
+        <f>AB44</f>
         <v>11355220</v>
       </c>
     </row>
@@ -15788,15 +15788,15 @@
         <v>45</v>
       </c>
       <c r="B117" s="9">
-        <f t="shared" si="27"/>
+        <f>F45</f>
         <v>8884195</v>
       </c>
       <c r="C117" s="9">
-        <f t="shared" si="28"/>
+        <f>Q45</f>
         <v>13400481</v>
       </c>
       <c r="D117" s="9">
-        <f t="shared" si="29"/>
+        <f>AB45</f>
         <v>19650139</v>
       </c>
     </row>
@@ -15805,15 +15805,15 @@
         <v>46</v>
       </c>
       <c r="B118" s="9">
-        <f t="shared" si="27"/>
+        <f>F46</f>
         <v>15043713</v>
       </c>
       <c r="C118" s="9">
-        <f t="shared" si="28"/>
+        <f>Q46</f>
         <v>23304696</v>
       </c>
       <c r="D118" s="9">
-        <f t="shared" si="29"/>
+        <f>AB46</f>
         <v>33210908</v>
       </c>
     </row>
@@ -15822,15 +15822,15 @@
         <v>47</v>
       </c>
       <c r="B119" s="9">
-        <f t="shared" si="27"/>
+        <f>F47</f>
         <v>10496859</v>
       </c>
       <c r="C119" s="9">
-        <f t="shared" si="28"/>
+        <f>Q47</f>
         <v>15855324</v>
       </c>
       <c r="D119" s="9">
-        <f t="shared" si="29"/>
+        <f>AB47</f>
         <v>22787977</v>
       </c>
     </row>
@@ -15877,15 +15877,15 @@
         <v>40</v>
       </c>
       <c r="B137" s="9">
-        <f t="shared" ref="B137:B144" si="30">B40</f>
+        <f t="shared" ref="B137:B144" si="24">B40</f>
         <v>174630</v>
       </c>
       <c r="C137" s="9">
-        <f t="shared" ref="C137:C144" si="31">M40</f>
+        <f t="shared" ref="C137:C144" si="25">M40</f>
         <v>265644</v>
       </c>
       <c r="D137" s="9">
-        <f t="shared" ref="D137:D144" si="32">X40</f>
+        <f t="shared" ref="D137:D144" si="26">X40</f>
         <v>393909</v>
       </c>
     </row>
@@ -15894,15 +15894,15 @@
         <v>41</v>
       </c>
       <c r="B138" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>204789</v>
       </c>
       <c r="C138" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>302348</v>
       </c>
       <c r="D138" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>440794</v>
       </c>
     </row>
@@ -15911,15 +15911,15 @@
         <v>42</v>
       </c>
       <c r="B139" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>313699</v>
       </c>
       <c r="C139" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>494697</v>
       </c>
       <c r="D139" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>742969</v>
       </c>
     </row>
@@ -15928,15 +15928,15 @@
         <v>44</v>
       </c>
       <c r="B140" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>381023</v>
       </c>
       <c r="C140" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>571673</v>
       </c>
       <c r="D140" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>832945</v>
       </c>
     </row>
@@ -15945,15 +15945,15 @@
         <v>43</v>
       </c>
       <c r="B141" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>206536</v>
       </c>
       <c r="C141" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>304275</v>
       </c>
       <c r="D141" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>441103</v>
       </c>
     </row>
@@ -15962,15 +15962,15 @@
         <v>45</v>
       </c>
       <c r="B142" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>313437</v>
       </c>
       <c r="C142" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>494491</v>
       </c>
       <c r="D142" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>742886</v>
       </c>
     </row>
@@ -15979,15 +15979,15 @@
         <v>46</v>
       </c>
       <c r="B143" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>556098</v>
       </c>
       <c r="C143" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>835669</v>
       </c>
       <c r="D143" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>1260367</v>
       </c>
     </row>
@@ -15996,15 +15996,15 @@
         <v>47</v>
       </c>
       <c r="B144" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="24"/>
         <v>411522</v>
       </c>
       <c r="C144" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="25"/>
         <v>605871</v>
       </c>
       <c r="D144" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="26"/>
         <v>881236</v>
       </c>
     </row>
@@ -16046,15 +16046,15 @@
         <v>40</v>
       </c>
       <c r="B152" s="9">
-        <f t="shared" ref="B152:B159" si="33">E40</f>
+        <f t="shared" ref="B152:B159" si="27">E40</f>
         <v>174292</v>
       </c>
       <c r="C152" s="9">
-        <f t="shared" ref="C152:C159" si="34">P40</f>
+        <f t="shared" ref="C152:C159" si="28">P40</f>
         <v>265204</v>
       </c>
       <c r="D152" s="9">
-        <f t="shared" ref="D152:D159" si="35">AA40</f>
+        <f t="shared" ref="D152:D159" si="29">AA40</f>
         <v>393232</v>
       </c>
     </row>
@@ -16063,15 +16063,15 @@
         <v>41</v>
       </c>
       <c r="B153" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>204456</v>
       </c>
       <c r="C153" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>301928</v>
       </c>
       <c r="D153" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>440344</v>
       </c>
     </row>
@@ -16080,15 +16080,15 @@
         <v>42</v>
       </c>
       <c r="B154" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>313052</v>
       </c>
       <c r="C154" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>491640</v>
       </c>
       <c r="D154" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>740328</v>
       </c>
     </row>
@@ -16097,15 +16097,15 @@
         <v>44</v>
       </c>
       <c r="B155" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>380652</v>
       </c>
       <c r="C155" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>568804</v>
       </c>
       <c r="D155" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>831368</v>
       </c>
     </row>
@@ -16114,15 +16114,15 @@
         <v>43</v>
       </c>
       <c r="B156" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>206384</v>
       </c>
       <c r="C156" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>303864</v>
       </c>
       <c r="D156" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>440800</v>
       </c>
     </row>
@@ -16131,15 +16131,15 @@
         <v>45</v>
       </c>
       <c r="B157" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>313024</v>
       </c>
       <c r="C157" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>492412</v>
       </c>
       <c r="D157" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>740580</v>
       </c>
     </row>
@@ -16148,15 +16148,15 @@
         <v>46</v>
       </c>
       <c r="B158" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>555648</v>
       </c>
       <c r="C158" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>834952</v>
       </c>
       <c r="D158" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>1259236</v>
       </c>
     </row>
@@ -16165,15 +16165,15 @@
         <v>47</v>
       </c>
       <c r="B159" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="27"/>
         <v>411220</v>
       </c>
       <c r="C159" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="28"/>
         <v>605476</v>
       </c>
       <c r="D159" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="29"/>
         <v>880396</v>
       </c>
     </row>

</xml_diff>